<commit_message>
big refactor, remade equation struct and made statistics algorithm a lot faster when using intermediates/probability_maps
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\totte\Documents\Projekt\minesweeper-probability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FFE32BD-9555-475E-A470-E039F28CC35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CABCABF-FEFB-4342-8D93-B745C93FF46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{571CE61A-5902-42CA-8033-A209C05CB203}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
   <si>
     <t>winrate</t>
   </si>
@@ -57,13 +57,55 @@
   </si>
   <si>
     <t>95% error</t>
+  </si>
+  <si>
+    <t>Same value strategy</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Corner + Perimeter</t>
+  </si>
+  <si>
+    <t>Processing time</t>
+  </si>
+  <si>
+    <t>Verify mrgris.com results</t>
+  </si>
+  <si>
+    <t>30m17.995s</t>
+  </si>
+  <si>
+    <t>Test Etas</t>
+  </si>
+  <si>
+    <t>17m24.160s</t>
+  </si>
+  <si>
+    <t>15m4.374s</t>
+  </si>
+  <si>
+    <t>14m25.339s</t>
+  </si>
+  <si>
+    <t>18m1.675s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +119,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -86,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -94,12 +152,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -118,7 +197,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -434,115 +513,436 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C809CD2D-D4F9-4B8B-98AE-B9843B295B39}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="B2:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="19.08984375" customWidth="1"/>
+    <col min="3" max="3" width="18.90625" customWidth="1"/>
     <col min="5" max="5" width="10.6328125" customWidth="1"/>
     <col min="6" max="6" width="15.26953125" customWidth="1"/>
     <col min="7" max="7" width="14.54296875" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.5">
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="4">
         <v>10000</v>
       </c>
-      <c r="F2">
-        <f>1.96*SQRT(A2 * (1 - A2) / E2)</f>
-        <v>9.5231799394949988E-3</v>
-      </c>
-      <c r="G2">
-        <f>ROUND(A2 - F2, 4)</f>
-        <v>0.3725</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>0.39079999999999998</v>
-      </c>
-      <c r="B3">
+      <c r="K4" s="2">
+        <f>1.96*SQRT(H4 * (1 - H4) / J4)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <f>ROUND(H4 - K4, 4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="4">
+        <v>10000</v>
+      </c>
+      <c r="K5" s="2">
+        <f>1.96*SQRT(H5 * (1 - H5) / J5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <f>ROUND(H5 - K5, 4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="4">
+        <v>10000</v>
+      </c>
+      <c r="K6" s="2">
+        <f>1.96*SQRT(H6 * (1 - H6) / J6)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <f>ROUND(H6 - K6, 4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>0.37949300000000002</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="K7" s="2">
+        <f>1.96*SQRT(H7 * (1 - H7) / J7)</f>
+        <v>9.5111120623855632E-4</v>
+      </c>
+      <c r="L7" s="2">
+        <f>ROUND(H7 - K7, 4)</f>
+        <v>0.3785</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="2:12" ht="21" x14ac:dyDescent="0.5">
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
+        <v>0.37949300000000002</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="K11" s="2">
+        <f>1.96*SQRT(H11 * (1 - H11) / J11)</f>
+        <v>9.5111120623855632E-4</v>
+      </c>
+      <c r="L11" s="2">
+        <f>ROUND(H11 - K11, 4)</f>
+        <v>0.3785</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2">
         <v>0.25</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>10000</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F4" si="0">1.96*SQRT(A3 * (1 - A3) / E3)</f>
-        <v>9.5634214744305807E-3</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G4" si="1">ROUND(A3 - F3, 4)</f>
-        <v>0.38119999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>0.39</v>
-      </c>
-      <c r="B4">
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2">
+        <v>0.3911</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="4">
+        <v>100000</v>
+      </c>
+      <c r="K12" s="2">
+        <f>1.96*SQRT(H12 * (1 - H12) / J12)</f>
+        <v>3.024634951302388E-3</v>
+      </c>
+      <c r="L12" s="2">
+        <f>ROUND(H12 - K12, 4)</f>
+        <v>0.3881</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2">
+        <v>0.39388000000000001</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="4">
+        <v>100000</v>
+      </c>
+      <c r="K13" s="2">
+        <f>1.96*SQRT(H13 * (1 - H13) / J13)</f>
+        <v>3.0284286301264555E-3</v>
+      </c>
+      <c r="L13" s="2">
+        <f>ROUND(H13 - K13, 4)</f>
+        <v>0.39090000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2">
         <v>0.75</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>10000</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>9.5598987442336442E-3</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="1"/>
-        <v>0.38040000000000002</v>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2">
+        <v>0.39223000000000002</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="4">
+        <v>100000</v>
+      </c>
+      <c r="K14" s="2">
+        <f>1.96*SQRT(H14 * (1 - H14) / J14)</f>
+        <v>3.0261893943825786E-3</v>
+      </c>
+      <c r="L14" s="2">
+        <f>ROUND(H14 - K14, 4)</f>
+        <v>0.38919999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2">
+        <v>0.34184999999999999</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="4">
+        <v>100000</v>
+      </c>
+      <c r="K15" s="2">
+        <f>1.96*SQRT(H15 * (1 - H15) / J15)</f>
+        <v>2.9399253720528351E-3</v>
+      </c>
+      <c r="L15" s="2">
+        <f>ROUND(H15 - K15, 4)</f>
+        <v>0.33889999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="4">
+        <v>100000</v>
+      </c>
+      <c r="K16" s="2">
+        <f>1.96*SQRT(H16 * (1 - H16) / J16)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <f>ROUND(H16 - K16, 4)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>